<commit_message>
fix: add force migrate in build script
</commit_message>
<xml_diff>
--- a/cypress/downloads/data-tugas-akhir-mahasiswa.xlsx
+++ b/cypress/downloads/data-tugas-akhir-mahasiswa.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
   <si>
     <t>NIM</t>
   </si>
@@ -29,6 +29,138 @@
     <t>Status</t>
   </si>
   <si>
+    <t>laksmiwati.bahuwarna</t>
+  </si>
+  <si>
+    <t>Darsirah Saefullah</t>
+  </si>
+  <si>
+    <t>D2 Pengembangan Piranti Lunak Situs</t>
+  </si>
+  <si>
+    <t>Belum Dikumpulkan</t>
+  </si>
+  <si>
+    <t>wiswahyudi</t>
+  </si>
+  <si>
+    <t>Calista Kuswoyo</t>
+  </si>
+  <si>
+    <t>winarsih.mursita</t>
+  </si>
+  <si>
+    <t>Tomi Damanik</t>
+  </si>
+  <si>
+    <t>ardianto.kamal</t>
+  </si>
+  <si>
+    <t>Jelita Kuswoyo</t>
+  </si>
+  <si>
+    <t>D4 Teknik Informatika</t>
+  </si>
+  <si>
+    <t>gambira10</t>
+  </si>
+  <si>
+    <t>Ganep Sihotang</t>
+  </si>
+  <si>
+    <t>sastuti</t>
+  </si>
+  <si>
+    <t>Tina Pertiwi</t>
+  </si>
+  <si>
+    <t>sinaga.labuh</t>
+  </si>
+  <si>
+    <t>Violet Prabowo</t>
+  </si>
+  <si>
+    <t>lsitompul</t>
+  </si>
+  <si>
+    <t>Suci Tarihoran</t>
+  </si>
+  <si>
+    <t>limar.nuraini</t>
+  </si>
+  <si>
+    <t>Aditya Tarihoran</t>
+  </si>
+  <si>
+    <t>maria53</t>
+  </si>
+  <si>
+    <t>Jarwadi Saragih</t>
+  </si>
+  <si>
+    <t>darimin63</t>
+  </si>
+  <si>
+    <t>Soleh Halimah</t>
+  </si>
+  <si>
+    <t>natalia33</t>
+  </si>
+  <si>
+    <t>Ellis Andriani</t>
+  </si>
+  <si>
+    <t>uwais.fathonah</t>
+  </si>
+  <si>
+    <t>Arsipatra Fujiati</t>
+  </si>
+  <si>
+    <t>yosef.hutasoit</t>
+  </si>
+  <si>
+    <t>Estiono Yuniar</t>
+  </si>
+  <si>
+    <t>prasasta.kusuma</t>
+  </si>
+  <si>
+    <t>Reksa Marpaung</t>
+  </si>
+  <si>
+    <t>heryanto38</t>
+  </si>
+  <si>
+    <t>Cayadi Adriansyah</t>
+  </si>
+  <si>
+    <t>kmarbun</t>
+  </si>
+  <si>
+    <t>Daliono Padmasari</t>
+  </si>
+  <si>
+    <t>omansur</t>
+  </si>
+  <si>
+    <t>Ibun Uyainah</t>
+  </si>
+  <si>
+    <t>satya.novitasari</t>
+  </si>
+  <si>
+    <t>Legawa Pratiwi</t>
+  </si>
+  <si>
+    <t>prima86</t>
+  </si>
+  <si>
+    <t>Shania Wacana</t>
+  </si>
+  <si>
+    <t>fahmi alfarizi</t>
+  </si>
+  <si>
     <t>susipujiastuti</t>
   </si>
   <si>
@@ -48,6 +180,12 @@
   </si>
   <si>
     <t>D4 Sistem Informasi Bisnis</t>
+  </si>
+  <si>
+    <t>farhan12</t>
+  </si>
+  <si>
+    <t>Farhan Asyam</t>
   </si>
   <si>
     <t>adesusilo</t>
@@ -393,7 +531,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +575,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -445,16 +583,324 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>2131762099</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>